<commit_message>
Fix bug- HS-Thị trường- Loại tiền-D_M_Y
</commit_message>
<xml_diff>
--- a/DongAERP/Content/Report/ReportHS/ReportHSCompare.xlsx
+++ b/DongAERP/Content/Report/ReportHS/ReportHSCompare.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DongAERP\DongAERP\Content\Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DongAERP\DongAERP\Content\Report\ReportHS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FA5D05-C2C7-47EB-AACB-BE0D4C2B7835}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29386FD7-1791-413D-A782-B592089025BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FDADBC8A-6B6C-45FD-98E5-87326587A42E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FDADBC8A-6B6C-45FD-98E5-87326587A42E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>BÁO CÁO TỔNG HỢP - LOẠI HÌNH DỊCH VỤ</t>
   </si>
@@ -41,34 +41,28 @@
     <t>Đơn vị:</t>
   </si>
   <si>
-    <t>Doanh số chi quầy</t>
-  </si>
-  <si>
-    <t>Doanh số chi nhà</t>
-  </si>
-  <si>
-    <t>Doanh số chi chuyển khoản</t>
-  </si>
-  <si>
-    <t>Tổng doanh số</t>
-  </si>
-  <si>
-    <t>Triệu USD</t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
-    <t>chi quầy</t>
-  </si>
-  <si>
-    <t>chi nhà</t>
-  </si>
-  <si>
-    <t>chi CK</t>
-  </si>
-  <si>
     <t>Tổng</t>
+  </si>
+  <si>
+    <t>Hồ sơ chi quầy</t>
+  </si>
+  <si>
+    <t>Hồ sơ chi nhà</t>
+  </si>
+  <si>
+    <t>Hồ sơ chuyển khoản</t>
+  </si>
+  <si>
+    <t>Chi quầy</t>
+  </si>
+  <si>
+    <t>Chi nhà</t>
+  </si>
+  <si>
+    <t>Chi CK</t>
   </si>
 </sst>
 </file>
@@ -154,14 +148,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -479,45 +473,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C3B6D35-F82E-4989-A479-5B01F28891A5}">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S35" sqref="S35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="17" max="17" width="17" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.5703125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-    </row>
-    <row r="2" spans="1:21" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+    </row>
+    <row r="2" spans="1:21" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -540,57 +534,52 @@
       <c r="T3" s="7"/>
       <c r="U3" s="7"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="L5" s="1"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="S6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S6" s="1"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="P7" s="3"/>
       <c r="Q7" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="T7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="S7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="T7" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="16:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="16:20" x14ac:dyDescent="0.3">
       <c r="R34"/>
       <c r="S34" s="1" t="s">
         <v>1</v>
       </c>
       <c r="T34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="16:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="P35" s="8"/>
+      <c r="Q35" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="35" spans="16:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="P35" s="9"/>
-      <c r="Q35" s="10" t="s">
+      <c r="R35" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="R35" s="10" t="s">
+      <c r="S35" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="S35" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="T35" s="10" t="s">
-        <v>11</v>
+      <c r="T35" s="9" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>